<commit_message>
More functionality, data and tests.
git-svn-id: file:///home/git/hedgehog.fhcrc.org/bioconductor/trunk/madman/Rpacks/flowQB@118028 bc3139a8-67e5-0310-9ffc-ced21a209358
</commit_message>
<xml_diff>
--- a/inst/extdata/example1/140126_InstEval_Stanford_LSRIIA2.xlsx
+++ b/inst/extdata/example1/140126_InstEval_Stanford_LSRIIA2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="250" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="224">
   <si>
     <t>140126 InstEvalTemplate.xls</t>
   </si>
@@ -161,10 +161,13 @@
     <t>Folder name</t>
   </si>
   <si>
-    <t>SU-2B</t>
-  </si>
-  <si>
-    <t>OtherTests</t>
+    <t>SU_2B</t>
+  </si>
+  <si>
+    <t>Other_Tests</t>
+  </si>
+  <si>
+    <t>LED_Series</t>
   </si>
   <si>
     <t>File Name</t>
@@ -1016,8 +1019,8 @@
   </sheetPr>
   <dimension ref="B2:U189"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R19" activeCellId="0" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1311,7 +1314,7 @@
         <v>49</v>
       </c>
       <c r="S18" s="0" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="U18" s="0" t="s">
         <v>36</v>
@@ -1319,63 +1322,63 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O19" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P19" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="Q19" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R19" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S19" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="U19" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>12</v>
@@ -1422,7 +1425,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>15</v>
@@ -1469,7 +1472,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D22" s="11" t="n">
         <v>2</v>
@@ -1525,156 +1528,156 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L23" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H24" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="J24" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="I24" s="12" t="s">
+      <c r="K24" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="J24" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="K24" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="L24" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H25" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J25" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="I25" s="12" t="s">
+      <c r="K25" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="J25" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="K25" s="12" t="s">
-        <v>80</v>
-      </c>
       <c r="L25" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M25" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G26" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="H26" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I26" s="12" t="s">
-        <v>84</v>
-      </c>
       <c r="J26" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L26" s="12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M26" s="15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
@@ -1685,16 +1688,16 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
       <c r="G28" s="17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
@@ -1705,76 +1708,76 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>20</v>
@@ -1809,10 +1812,10 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="20"/>
@@ -1828,7 +1831,7 @@
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="22"/>
       <c r="C46" s="23" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D46" s="23"/>
       <c r="E46" s="23"/>
@@ -1844,7 +1847,7 @@
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="22"/>
       <c r="C47" s="23" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D47" s="23"/>
       <c r="E47" s="23"/>
@@ -1860,7 +1863,7 @@
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="22"/>
       <c r="C48" s="23" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D48" s="23"/>
       <c r="E48" s="23"/>
@@ -1876,7 +1879,7 @@
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22"/>
       <c r="C49" s="23" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D49" s="23"/>
       <c r="E49" s="23"/>
@@ -1892,7 +1895,7 @@
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="25"/>
       <c r="C50" s="26" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D50" s="26"/>
       <c r="E50" s="26"/>
@@ -1908,7 +1911,7 @@
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="25"/>
       <c r="C51" s="26" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D51" s="26"/>
       <c r="E51" s="26"/>
@@ -1924,7 +1927,7 @@
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="25"/>
       <c r="C52" s="26" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D52" s="26"/>
       <c r="E52" s="26"/>
@@ -1939,305 +1942,305 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="28" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C88" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C89" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C95" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C108" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C109" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2245,151 +2248,151 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C116" s="6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C118" s="6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C121" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C122" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C123" s="6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C124" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C125" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C126" s="6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C127" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C128" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C132" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C133" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C134" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C135" s="6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C136" s="6" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C137" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C138" s="6" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C140" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C141" s="6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C142" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C143" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2397,100 +2400,100 @@
         <v>34</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C146" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C147" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C148" s="6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C149" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C150" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C151" s="6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C152" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C153" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C154" s="6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C155" s="6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C156" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C157" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C158" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C159" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C160" s="6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C161" s="6" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C162" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="28" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D164" s="6" t="s">
         <v>20</v>
@@ -2525,68 +2528,68 @@
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C166" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C167" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C168" s="6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C169" s="6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C170" s="6" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B172" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C173" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C174" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C175" s="6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C176" s="6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C177" s="6" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,45 +2597,45 @@
         <v>34</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C180" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C181" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C182" s="6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C183" s="6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C184" s="6" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B186" s="28" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B187" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C187" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D187" s="20"/>
       <c r="E187" s="20"/>
@@ -2647,10 +2650,10 @@
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B188" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C188" s="30" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D188" s="23"/>
       <c r="E188" s="23"/>
@@ -2668,7 +2671,7 @@
         <v>34</v>
       </c>
       <c r="C189" s="31" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D189" s="26"/>
       <c r="E189" s="26"/>

</xml_diff>